<commit_message>
Updating tract script and notebooks
</commit_message>
<xml_diff>
--- a/DataDictionaries/DataDictionaries.xlsx
+++ b/DataDictionaries/DataDictionaries.xlsx
@@ -5,16 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tylermatteo/projects/lead-paint-data-scripts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tylermatteo/projects/USI_Lead_Paint_Hazard/DataDictionaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1302E46-F8A1-E84D-83AE-7B000D94E26E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B365D7-98D0-6D4A-AEAB-5E862AEFC454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21340" xr2:uid="{A2623886-6688-9C4F-9F16-A084D976F829}"/>
+    <workbookView xWindow="2080" yWindow="500" windowWidth="38400" windowHeight="21340" xr2:uid="{A2623886-6688-9C4F-9F16-A084D976F829}"/>
   </bookViews>
   <sheets>
     <sheet name="Tax Lots" sheetId="1" r:id="rId1"/>
     <sheet name="Census Tracts" sheetId="2" r:id="rId2"/>
+    <sheet name="Complaints" sheetId="3" r:id="rId3"/>
+    <sheet name="Problems" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="146">
   <si>
     <t>Property</t>
   </si>
@@ -361,13 +363,133 @@
   </si>
   <si>
     <t>Census Tract Data Dictionary</t>
+  </si>
+  <si>
+    <t>lots</t>
+  </si>
+  <si>
+    <t>Total number of tax lots containing at least 3 rental units and built before 1960</t>
+  </si>
+  <si>
+    <t>all_lots</t>
+  </si>
+  <si>
+    <t>Total number of tax lots containing at least 3 rental units (including those built after 1960)</t>
+  </si>
+  <si>
+    <t>percent_lot_pre_1960</t>
+  </si>
+  <si>
+    <t>Percentage of relevant lots that were built before 1960</t>
+  </si>
+  <si>
+    <t>percent_pre_1960</t>
+  </si>
+  <si>
+    <t>Percentage of relevant housing units that are in a building before 1960</t>
+  </si>
+  <si>
+    <t>1 the inspector was able to inspect all associated problems and issued no violations, else 0</t>
+  </si>
+  <si>
+    <t>integer (binary)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no_violation </t>
+  </si>
+  <si>
+    <t>1 if a violation was issued for at least one of the associated problems for this complaint, else 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">violation </t>
+  </si>
+  <si>
+    <t>1 if the inspector was not able to gain entry to inspect at least one of the associated problems, else 0</t>
+  </si>
+  <si>
+    <t>no_entry</t>
+  </si>
+  <si>
+    <t>Total number of problems associated with this complaint</t>
+  </si>
+  <si>
+    <t>problems</t>
+  </si>
+  <si>
+    <t>Number of problems for this compalint wherein a violation was issued</t>
+  </si>
+  <si>
+    <t>Number of problems for this complaint wherein the problem was inspected and no violation was issued</t>
+  </si>
+  <si>
+    <t>Number of problems for this complaint wherein the inspector was not able to gain entry</t>
+  </si>
+  <si>
+    <t>Date status code was last updated</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>status_date</t>
+  </si>
+  <si>
+    <t>Current status of complaint - "OPEN" or "CLOSE"</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>Date when the complaint was received </t>
+  </si>
+  <si>
+    <t>received_date</t>
+  </si>
+  <si>
+    <t>Borough block lot identifier</t>
+  </si>
+  <si>
+    <t>Unique identifier given to a building record </t>
+  </si>
+  <si>
+    <t>building_id</t>
+  </si>
+  <si>
+    <t>Unique identifier of the complaint this problem is associated with</t>
+  </si>
+  <si>
+    <t>complaint_id</t>
+  </si>
+  <si>
+    <t>Complaint Data Dictionary</t>
+  </si>
+  <si>
+    <t>Result of problem - "no_entry", "violation", or "no_violation"</t>
+  </si>
+  <si>
+    <t>result</t>
+  </si>
+  <si>
+    <t>Identifier for corresponding problem. Note there is a 1-to-n relationship between complaints and problems. Each complaint is associated with one or more problems</t>
+  </si>
+  <si>
+    <t>Unique identifier for problem</t>
+  </si>
+  <si>
+    <t>problem_id</t>
+  </si>
+  <si>
+    <t>Problems Data Dictionary</t>
+  </si>
+  <si>
+    <t>See description in Census Tract dictionary</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -386,6 +508,19 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -411,7 +546,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -424,6 +559,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -738,9 +874,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD91E214-6951-5B40-B4F3-B373617BB3EB}">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1127,6 +1265,116 @@
         <v>69</v>
       </c>
     </row>
+    <row r="37" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>70</v>
+      </c>
+      <c r="B37" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>72</v>
+      </c>
+      <c r="B39" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>73</v>
+      </c>
+      <c r="B40" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>75</v>
+      </c>
+      <c r="B42" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>76</v>
+      </c>
+      <c r="B43" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>77</v>
+      </c>
+      <c r="B44" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>78</v>
+      </c>
+      <c r="B45" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>79</v>
+      </c>
+      <c r="B46" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1135,9 +1383,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D6AC60F-A593-D04D-9887-70CC4FB31387}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView zoomScale="185" zoomScaleNormal="185" workbookViewId="0"/>
+    <sheetView zoomScale="185" zoomScaleNormal="185" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:C13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1532,8 +1782,314 @@
         <v>92</v>
       </c>
     </row>
+    <row r="38" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{523AF64D-80D4-0C45-AC63-3953D3FF6815}">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView zoomScale="275" zoomScaleNormal="275" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B14" t="s">
+        <v>115</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>116</v>
+      </c>
+      <c r="B16" t="s">
+        <v>115</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AA3FC57-9FC0-8849-9A1D-0F0A50AF97D4}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>